<commit_message>
Adjust Database to Boyce-Codd Normal Form
</commit_message>
<xml_diff>
--- a/Excel and CSV Datenbank/Fachbereiche.xlsx
+++ b/Excel and CSV Datenbank/Fachbereiche.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kien\Desktop\Seminar\Datenbank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kien\Desktop\Seminar\Excel and CSV Datenbank\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -150,22 +150,13 @@
   </si>
   <si>
     <t>FBNr</t>
-  </si>
-  <si>
-    <t>Infrastruktur</t>
-  </si>
-  <si>
-    <t>Mensa</t>
-  </si>
-  <si>
-    <t>Mensa, Bibliothek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,18 +164,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -194,13 +228,141 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -214,16 +376,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0">
-  <autoFilter ref="A1:D14"/>
-  <sortState ref="A2:C14">
-    <sortCondition ref="A1:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C14" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C14"/>
+  <sortState ref="A2:D17">
+    <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="FBNr"/>
-    <tableColumn id="2" name="Bezeichnung"/>
-    <tableColumn id="3" name="Ort"/>
-    <tableColumn id="7" name="Infrastruktur"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="FBNr" dataDxfId="2"/>
+    <tableColumn id="2" name="Bezeichnung" dataDxfId="1"/>
+    <tableColumn id="3" name="Ort" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,213 +653,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>